<commit_message>
code changes and ppt
code changes and ppt
</commit_message>
<xml_diff>
--- a/NetbeansProjects/Parade Route Dynamic Graph/Input Route Data Template.xlsx
+++ b/NetbeansProjects/Parade Route Dynamic Graph/Input Route Data Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\Data-Structure-Design\NetbeansProjects\Parade Route Dynamic Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F75ED-945A-4437-8C7A-01752FF206B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF015A26-A8A1-48D2-9CD7-2FCEF06535E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" xr2:uid="{B96E8E76-8475-4F7C-8615-E3CDEC40FC00}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>시위대명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,6 +121,34 @@
   </si>
   <si>
     <t>한국은행→눈스퀘어→을지1→광교→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속도 * 총시간 = 총거리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">45 * 80 = 3600 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>29 * 120 = 3480</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 * 120 = 1440</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 * 210 = 6300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21 * 160 = 3360</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 * 150 = 2550</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,15 +650,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F354919E-7C38-4968-8A20-CB1CE7FDA2C4}">
-  <dimension ref="B1:F11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
@@ -639,10 +667,10 @@
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
@@ -651,14 +679,14 @@
       <c r="E2" s="12"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
@@ -667,7 +695,10 @@
       <c r="E4" s="10"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -681,7 +712,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -695,7 +729,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
@@ -709,7 +746,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
@@ -723,7 +763,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
@@ -737,7 +780,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
@@ -751,7 +797,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>

</xml_diff>